<commit_message>
Revert "Revert "Bütçe Düzenlemesi""
This reverts commit 50b0fbbb4955f335c51b9483fd266821a9a06844.
</commit_message>
<xml_diff>
--- a/BBM487-2-Bütçe.xlsx
+++ b/BBM487-2-Bütçe.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furkan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furkan\Desktop\yaz müh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roller" sheetId="1" r:id="rId1"/>
@@ -228,6 +228,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -237,8 +239,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -644,11 +644,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -701,7 +701,7 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>21127237</v>
       </c>
     </row>
@@ -712,7 +712,7 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>21027205</v>
       </c>
     </row>
@@ -723,7 +723,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>21127606</v>
       </c>
     </row>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,17 +762,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -837,16 +837,30 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="B4" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4000</v>
+      </c>
+      <c r="F4" s="5">
+        <v>6000</v>
+      </c>
+      <c r="G4" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
       <c r="I4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -930,15 +944,15 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -992,14 +1006,22 @@
       <c r="A14" s="2">
         <v>2</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
       <c r="G14" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1091,10 +1113,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -1119,7 +1141,7 @@
       </c>
       <c r="B24" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1128,7 +1150,7 @@
       </c>
       <c r="B25" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1137,7 +1159,7 @@
       </c>
       <c r="B26" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1146,7 +1168,7 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1155,7 +1177,7 @@
       </c>
       <c r="B28" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1164,7 +1186,7 @@
       </c>
       <c r="B29" s="5">
         <f t="shared" si="3"/>
-        <v>66000</v>
+        <v>32000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>